<commit_message>
added leetcode 11 water container solution, brute force and optimised
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhisingh/Documents/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16F72A54-96E8-9742-AEC5-CC89518D1613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074E95D7-5E76-224B-B33D-D3AF65C9E0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8320" yWindow="5700" windowWidth="20480" windowHeight="11360" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -207,6 +207,21 @@
   </si>
   <si>
     <t>tuple unpacking; create a in place modification by converting string to a list using function list(string)</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/container-with-most-water/submissions/1309600772?source=submission-ac</t>
+  </si>
+  <si>
+    <t>two pointer problem</t>
+  </si>
+  <si>
+    <t>Container with most water</t>
+  </si>
+  <si>
+    <t>medium</t>
   </si>
 </sst>
 </file>
@@ -252,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -275,12 +290,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -295,6 +321,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -313,10 +342,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -726,21 +751,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5180F1-9E51-5F4C-814F-CA142751DA71}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="85.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -753,8 +778,11 @@
       <c r="D1" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="E1" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -766,6 +794,23 @@
       </c>
       <c r="D2" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
leet code problem 283 and 605
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhisingh/Documents/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074E95D7-5E76-224B-B33D-D3AF65C9E0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DB94C1-1812-6646-B68E-100DDFCD9300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8320" yWindow="5700" windowWidth="20480" windowHeight="11360" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
   </bookViews>
@@ -754,7 +754,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated excel with latest info and added edge case to 'can place flowers'
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhisingh/Documents/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DB94C1-1812-6646-B68E-100DDFCD9300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BF3A30-A176-AD49-B986-2CD8BAA21E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8320" yWindow="5700" windowWidth="20480" windowHeight="11360" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
+    <workbookView xWindow="0" yWindow="1440" windowWidth="20480" windowHeight="11360" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Description</t>
   </si>
@@ -222,6 +222,21 @@
   </si>
   <si>
     <t>medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">easy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">move zeroes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">can place flowers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">edge cases to note </t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/can-place-flowers/submissions/1316656978?envType=study-plan-v2&amp;envId=leetcode-75</t>
   </si>
 </sst>
 </file>
@@ -306,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -326,6 +341,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -751,10 +767,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5180F1-9E51-5F4C-814F-CA142751DA71}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -813,7 +829,41 @@
         <v>26</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>283</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>605</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{AFD2A373-AB20-B448-BCD5-53AEFCF5F304}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
leetcode problem 933; queue problem using deque() class
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhisingh/Documents/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BF3A30-A176-AD49-B986-2CD8BAA21E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4094FE4-8A97-754F-9385-AF542199E6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1440" windowWidth="20480" windowHeight="11360" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
+    <workbookView xWindow="100" yWindow="1060" windowWidth="20480" windowHeight="11360" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Description</t>
   </si>
@@ -237,6 +237,18 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/can-place-flowers/submissions/1316656978?envType=study-plan-v2&amp;envId=leetcode-75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maximum average subarray </t>
+  </si>
+  <si>
+    <t>sliding window</t>
+  </si>
+  <si>
+    <t>Maximum Number of Vowels in a Substring of Given Length</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-number-of-vowels-in-a-substring-of-given-length/submissions/1321986754?envType=study-plan-v2&amp;envId=leetcode-75</t>
   </si>
 </sst>
 </file>
@@ -321,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -342,6 +354,15 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -767,28 +788,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5180F1-9E51-5F4C-814F-CA142751DA71}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="85.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -798,71 +819,101 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="9">
         <v>345</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="9">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="9">
         <v>283</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="9">
         <v>605</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="9">
+        <v>643</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1456</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{AFD2A373-AB20-B448-BCD5-53AEFCF5F304}"/>
+    <hyperlink ref="E7" r:id="rId2" xr:uid="{B5C38884-E7EF-DE48-A455-FB030602E1F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
deque problems. no: 649 and 933
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhisingh/Documents/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4094FE4-8A97-754F-9385-AF542199E6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D8D1F2-76BD-8B4F-8D58-CA06FDDCE7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="1060" windowWidth="20480" windowHeight="11360" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="14360" windowHeight="17520" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Description</t>
   </si>
@@ -249,6 +249,21 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/maximum-number-of-vowels-in-a-substring-of-given-length/submissions/1321986754?envType=study-plan-v2&amp;envId=leetcode-75</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/dota2-senate/submissions/1323838952?envType=study-plan-v2&amp;envId=leetcode-75</t>
+  </si>
+  <si>
+    <t>deque(); algo is interesting keep in mind</t>
+  </si>
+  <si>
+    <t>Dota2 Senate</t>
+  </si>
+  <si>
+    <t>Number of Recent Calls</t>
+  </si>
+  <si>
+    <t>deque()</t>
   </si>
 </sst>
 </file>
@@ -333,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -362,6 +377,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -788,10 +809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5180F1-9E51-5F4C-814F-CA142751DA71}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -910,10 +931,42 @@
         <v>38</v>
       </c>
     </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="9">
+        <v>649</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="12">
+        <v>933</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{AFD2A373-AB20-B448-BCD5-53AEFCF5F304}"/>
     <hyperlink ref="E7" r:id="rId2" xr:uid="{B5C38884-E7EF-DE48-A455-FB030602E1F1}"/>
+    <hyperlink ref="B8" r:id="rId3" display="https://leetcode.com/problems/dota2-senate/" xr:uid="{20D44867-E4A6-0947-B21E-FB7519307C2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LL and string easy codes from Leetcode
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhisingh/Documents/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D8D1F2-76BD-8B4F-8D58-CA06FDDCE7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99498908-0214-944A-A788-E9A6EC8DFC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="14360" windowHeight="17520" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14360" windowHeight="11360" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>Description</t>
   </si>
@@ -264,6 +264,33 @@
   </si>
   <si>
     <t>deque()</t>
+  </si>
+  <si>
+    <t>Roman to Integer</t>
+  </si>
+  <si>
+    <t>logic is imp; if s[i] &lt; s[i+1] then subtract it</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/roman-to-integer/submissions/1329786926</t>
+  </si>
+  <si>
+    <t>Odd even Linked List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse Linked List </t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dictionary </t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queue </t>
   </si>
 </sst>
 </file>
@@ -348,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -377,12 +404,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -809,10 +830,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5180F1-9E51-5F4C-814F-CA142751DA71}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -820,10 +841,11 @@
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="85.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="85.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -833,14 +855,17 @@
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
@@ -850,11 +875,12 @@
       <c r="C2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>29</v>
       </c>
@@ -864,14 +890,15 @@
       <c r="C3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -881,11 +908,12 @@
       <c r="C4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>30</v>
       </c>
@@ -895,14 +923,15 @@
       <c r="C5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -912,9 +941,10 @@
       <c r="C6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>29</v>
       </c>
@@ -924,48 +954,103 @@
       <c r="C7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="9">
         <v>649</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="9">
         <v>933</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="9">
+        <v>328</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="9">
+        <v>206</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{AFD2A373-AB20-B448-BCD5-53AEFCF5F304}"/>
-    <hyperlink ref="E7" r:id="rId2" xr:uid="{B5C38884-E7EF-DE48-A455-FB030602E1F1}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{AFD2A373-AB20-B448-BCD5-53AEFCF5F304}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{B5C38884-E7EF-DE48-A455-FB030602E1F1}"/>
     <hyperlink ref="B8" r:id="rId3" display="https://leetcode.com/problems/dota2-senate/" xr:uid="{20D44867-E4A6-0947-B21E-FB7519307C2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
leet code 14; longest prefix
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhisingh/Documents/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99498908-0214-944A-A788-E9A6EC8DFC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C428B1-284C-674C-80FA-77EAFB5A4AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14360" windowHeight="11360" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
   <si>
     <t>Description</t>
   </si>
@@ -291,6 +291,18 @@
   </si>
   <si>
     <t xml:space="preserve">Queue </t>
+  </si>
+  <si>
+    <t>Longest common prefix</t>
+  </si>
+  <si>
+    <t>string manipulation</t>
+  </si>
+  <si>
+    <t>you an take any string in the list as a string to compare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/longest-common-prefix/submissions/1332877197 </t>
   </si>
 </sst>
 </file>
@@ -830,10 +842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5180F1-9E51-5F4C-814F-CA142751DA71}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,11 +1059,32 @@
         <v>51</v>
       </c>
     </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1" xr:uid="{AFD2A373-AB20-B448-BCD5-53AEFCF5F304}"/>
     <hyperlink ref="F7" r:id="rId2" xr:uid="{B5C38884-E7EF-DE48-A455-FB030602E1F1}"/>
     <hyperlink ref="B8" r:id="rId3" display="https://leetcode.com/problems/dota2-senate/" xr:uid="{20D44867-E4A6-0947-B21E-FB7519307C2F}"/>
+    <hyperlink ref="F13" r:id="rId4" xr:uid="{7593DB7E-C406-7A4E-A8D0-CF96B087638E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
leetcode problems and binary, bubble and count sort. Also, binary tree traversal - stack and recursive approach
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhisingh/Documents/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F36EB6-37E8-FD40-9DAA-2B6CF964CF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AB77D3-0AF6-784B-969D-FF7BA44FA441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13040" yWindow="3020" windowWidth="14360" windowHeight="11360" activeTab="1" xr2:uid="{A1ADDF95-ABF0-E247-829D-148524113CE2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
   <si>
     <t>Description</t>
   </si>
@@ -357,6 +357,30 @@
   </si>
   <si>
     <t>Product of Array Except</t>
+  </si>
+  <si>
+    <t>Successful Pairs of Spells and Potions</t>
+  </si>
+  <si>
+    <t>binary search ; sorting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check both sub mission. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/successful-pairs-of-spells-and-potions/submissions/1352861094?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>Leaf-Similar Trees</t>
+  </si>
+  <si>
+    <t>DFS binary Tree</t>
+  </si>
+  <si>
+    <t>recursive and stack approach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/leaf-similar-trees/submissions/1362715863?envType=study-plan-v2&amp;envId=leetcode-75 </t>
   </si>
 </sst>
 </file>
@@ -441,7 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -462,14 +486,8 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -911,18 +929,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5180F1-9E51-5F4C-814F-CA142751DA71}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="10" customWidth="1"/>
     <col min="5" max="5" width="85.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="138.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -931,13 +949,13 @@
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>49</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -948,30 +966,30 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="12">
         <v>345</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="12">
         <v>11</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F3" t="s">
@@ -979,30 +997,30 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="12">
         <v>283</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="12">
         <v>605</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1010,28 +1028,28 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>643</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="12">
         <v>1456</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="7" t="s">
@@ -1039,19 +1057,19 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="12">
         <v>649</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>40</v>
       </c>
       <c r="F8" t="s">
@@ -1059,36 +1077,36 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="12">
         <v>933</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="12">
         <v>13</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F10" t="s">
@@ -1096,47 +1114,47 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="12">
         <v>328</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>206</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <v>14</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>55</v>
       </c>
       <c r="F13" s="7" t="s">
@@ -1144,16 +1162,16 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="12">
         <v>20</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F14" s="7" t="s">
@@ -1161,16 +1179,16 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="12">
         <v>66</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>61</v>
       </c>
       <c r="E15" t="s">
@@ -1181,16 +1199,16 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="12">
         <v>26</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="10" t="s">
         <v>65</v>
       </c>
       <c r="F16" s="7" t="s">
@@ -1198,16 +1216,16 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="12">
         <v>392</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="10" t="s">
         <v>67</v>
       </c>
       <c r="F17" s="7" t="s">
@@ -1215,16 +1233,16 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="12">
         <v>374</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>69</v>
       </c>
       <c r="E18" t="s">
@@ -1235,25 +1253,65 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="12">
         <v>1207</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="10" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="12">
         <v>238</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="10" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="12">
+        <v>2300</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="12">
+        <v>872</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1267,6 +1325,8 @@
     <hyperlink ref="F15" r:id="rId7" xr:uid="{1DF272DE-02D9-C240-9C31-8AB1BA3DA57A}"/>
     <hyperlink ref="F17" r:id="rId8" xr:uid="{EF95C3CA-48BF-6C43-A84A-9C6F8E405F3B}"/>
     <hyperlink ref="F18" r:id="rId9" xr:uid="{72DD4FDC-572A-7A46-B54E-9C31DB146A26}"/>
+    <hyperlink ref="F21" r:id="rId10" xr:uid="{7902205A-A959-CD4B-BF06-66BECC9E14E7}"/>
+    <hyperlink ref="F22" r:id="rId11" xr:uid="{919BB68D-DF36-4B45-8D5E-37AC723C5EA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>